<commit_message>
plots for teh gates action and linear models of water quality
</commit_message>
<xml_diff>
--- a/fmwt_smscg results.xlsx
+++ b/fmwt_smscg results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/rosemary_hartman_water_ca_gov/Documents/salinity control gates/SMSCG/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhartman\OneDrive - California Department of Water Resources\salinity control gates\SMSCG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{0EF606B9-A019-4E19-A85A-728373D110D3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{D52194B4-1117-4F8C-8737-DE5709BC3BEA}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{0EF606B9-A019-4E19-A85A-728373D110D3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{84C6B1BF-C887-4364-9304-DCB1A0F85639}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{BA6B06F5-E2C1-4D63-BD0F-2C1F52EB90C8}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="35">
   <si>
     <t>Count model coefficients (negbin with log link):</t>
   </si>
@@ -117,6 +117,24 @@
   </si>
   <si>
     <t>&lt; 2e-16</t>
+  </si>
+  <si>
+    <t>Dry years, scaled covariates</t>
+  </si>
+  <si>
+    <t>Dry years</t>
+  </si>
+  <si>
+    <t>(Intercept)</t>
+  </si>
+  <si>
+    <t>Gate Ops</t>
+  </si>
+  <si>
+    <t>FMWT Index</t>
+  </si>
+  <si>
+    <t>Operating</t>
   </si>
 </sst>
 </file>
@@ -494,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39AA4E36-38D7-4612-B787-2F3E70F50049}">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:F45"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="Q55" sqref="Q55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,6 +855,11 @@
         <v>2</v>
       </c>
     </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>0</v>
@@ -1157,6 +1180,255 @@
       </c>
       <c r="E45" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+      <c r="B53" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53" t="s">
+        <v>4</v>
+      </c>
+      <c r="D53" t="s">
+        <v>5</v>
+      </c>
+      <c r="E53" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B54">
+        <v>0.46050000000000002</v>
+      </c>
+      <c r="C54">
+        <v>0.47120000000000001</v>
+      </c>
+      <c r="D54">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="E54">
+        <v>0.32850000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B55">
+        <v>-1.3132999999999999</v>
+      </c>
+      <c r="C55">
+        <v>0.58120000000000005</v>
+      </c>
+      <c r="D55">
+        <v>-2.2599999999999998</v>
+      </c>
+      <c r="E55">
+        <v>2.3800000000000002E-2</v>
+      </c>
+      <c r="F55" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B56">
+        <v>0.5272</v>
+      </c>
+      <c r="C56">
+        <v>0.23630000000000001</v>
+      </c>
+      <c r="D56">
+        <v>2.2309999999999999</v>
+      </c>
+      <c r="E56">
+        <v>2.5700000000000001E-2</v>
+      </c>
+      <c r="F56" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B57">
+        <v>-0.34489999999999998</v>
+      </c>
+      <c r="C57">
+        <v>0.22270000000000001</v>
+      </c>
+      <c r="D57">
+        <v>-1.5489999999999999</v>
+      </c>
+      <c r="E57">
+        <v>0.1215</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B58">
+        <v>0.28649999999999998</v>
+      </c>
+      <c r="C58">
+        <v>0.15620000000000001</v>
+      </c>
+      <c r="D58">
+        <v>1.8340000000000001</v>
+      </c>
+      <c r="E58">
+        <v>6.6600000000000006E-2</v>
+      </c>
+      <c r="F58" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B59">
+        <v>-0.1285</v>
+      </c>
+      <c r="C59">
+        <v>0.45629999999999998</v>
+      </c>
+      <c r="D59">
+        <v>-0.28199999999999997</v>
+      </c>
+      <c r="E59">
+        <v>0.77829999999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="1"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="2"/>
+      <c r="B62" t="s">
+        <v>3</v>
+      </c>
+      <c r="C62" t="s">
+        <v>4</v>
+      </c>
+      <c r="D62" t="s">
+        <v>5</v>
+      </c>
+      <c r="E62" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B63">
+        <v>-65.239999999999995</v>
+      </c>
+      <c r="C63">
+        <v>83.4</v>
+      </c>
+      <c r="D63">
+        <v>-0.78200000000000003</v>
+      </c>
+      <c r="E63">
+        <v>0.434</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B64">
+        <v>-189.06</v>
+      </c>
+      <c r="C64">
+        <v>233.06</v>
+      </c>
+      <c r="D64">
+        <v>-0.81100000000000005</v>
+      </c>
+      <c r="E64">
+        <v>0.41699999999999998</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B65">
+        <v>44.54</v>
+      </c>
+      <c r="C65">
+        <v>58.02</v>
+      </c>
+      <c r="D65">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="E65">
+        <v>0.443</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B66">
+        <v>-52.58</v>
+      </c>
+      <c r="C66">
+        <v>64.34</v>
+      </c>
+      <c r="D66">
+        <v>-0.81699999999999995</v>
+      </c>
+      <c r="E66">
+        <v>0.41399999999999998</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B67">
+        <v>-225.33</v>
+      </c>
+      <c r="C67">
+        <v>277.66000000000003</v>
+      </c>
+      <c r="D67">
+        <v>-0.81200000000000006</v>
+      </c>
+      <c r="E67">
+        <v>0.41699999999999998</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1166,24 +1438,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C65D496D98813D4DBEDE643E5807C583" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f70dc900201e4f91fd7f1b7c6e5e96bc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="d8e3e477-4a6b-4f2c-bc61-5e11693be0f9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="551e6a62a1345ad5670b0f55e5c5fd75" ns1:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1370,32 +1624,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63868AC1-93E0-4D93-A0B2-4B7B62452E48}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="d8e3e477-4a6b-4f2c-bc61-5e11693be0f9"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE3FE013-B488-418B-90CA-13071B113826}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{249DE725-CD7A-41C6-938F-1917B044ECA4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1412,4 +1659,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE3FE013-B488-418B-90CA-13071B113826}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63868AC1-93E0-4D93-A0B2-4B7B62452E48}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="d8e3e477-4a6b-4f2c-bc61-5e11693be0f9"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>